<commit_message>
added list of failed downloads. moved summary file to subdirectory based on list number.
</commit_message>
<xml_diff>
--- a/korbinian/settings/korbinian_run_settings_TMD_server.xlsx
+++ b/korbinian/settings/korbinian_run_settings_TMD_server.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
+    <workbookView xWindow="3090" yWindow="2895" windowWidth="14265" windowHeight="7920"/>
   </bookViews>
   <sheets>
     <sheet name="run_settings" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="204">
   <si>
     <t>uniprot_list</t>
   </si>
@@ -297,9 +297,6 @@
     <t>mp_smallest_bin</t>
   </si>
   <si>
-    <t>UniProt run settings</t>
-  </si>
-  <si>
     <t>SIMAP run settings</t>
   </si>
   <si>
@@ -540,6 +537,75 @@
     <t>slice_juxtamembrane_regions</t>
   </si>
   <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>add_user_subseqs</t>
+  </si>
+  <si>
+    <t>If "TRUE", user-based TMD or subsequences will be added from an external file (e.g. List12_SE_seqs).</t>
+  </si>
+  <si>
+    <t>OMPdb_extract_omp_IDs_from_nr_fasta</t>
+  </si>
+  <si>
+    <t>OMPdb_parse_OMPdb_all_selected_to_csv</t>
+  </si>
+  <si>
+    <t>OMPdb_get_omp_TM_indices_and_slice_from_summary_table</t>
+  </si>
+  <si>
+    <t>omp_nr_fasta</t>
+  </si>
+  <si>
+    <t>OMPdb_all_flatfile</t>
+  </si>
+  <si>
+    <t>OMPdb_summary_nr_csv</t>
+  </si>
+  <si>
+    <t>D:\Databases\OMPdb\20160819_OMPdb.30</t>
+  </si>
+  <si>
+    <t>omp_ID_nr_txt</t>
+  </si>
+  <si>
+    <t>omp_nr_fasta + "_IDS.txt"</t>
+  </si>
+  <si>
+    <t>r"D:\Databases\OMPdb\20160819_OMPdb.flat"</t>
+  </si>
+  <si>
+    <t>D:\Databases\OMPdb\rimma_orig\OMPdb_Selected_by_potential_IDs.csv</t>
+  </si>
+  <si>
+    <t>OMPdb_summary_csv_with_TM_seqs</t>
+  </si>
+  <si>
+    <t>D:\Databases\main\summaries\List05_summary.csv</t>
+  </si>
+  <si>
+    <t>e.g. D:\Databases\main\summaries\List05_summary.csv, final output CSV file that will be treated like a uniprot summary file for the rest of the korbinian scripts</t>
+  </si>
+  <si>
+    <t>Protein list settings (UniProt/OMPdb)</t>
+  </si>
+  <si>
+    <t>Protein list (UniProt) settings</t>
+  </si>
+  <si>
+    <t>Protein list (OMPdb) settings [for outer membrane protein analysis]</t>
+  </si>
+  <si>
+    <t>/nas</t>
+  </si>
+  <si>
+    <t>/nas/teeselab/mark/databases</t>
+  </si>
+  <si>
+    <t>/nas/teeselab/mark/files/main</t>
+  </si>
+  <si>
     <t>/nas/teeselab/programs/eaSimap.jar</t>
   </si>
   <si>
@@ -555,37 +621,19 @@
     <t>/nas/teeselab/mark/databases/homol</t>
   </si>
   <si>
-    <t>/nas/teeselab/mark/files/main</t>
-  </si>
-  <si>
-    <t>/nas/teeselab/mark/databases</t>
-  </si>
-  <si>
-    <t>/nas</t>
-  </si>
-  <si>
-    <t>java</t>
-  </si>
-  <si>
-    <t>insert\path\to\List01_uniprot_accessions.txt</t>
+    <t>path\to\List01_uniprot_accessions.txt</t>
   </si>
   <si>
     <t>Mark Teese</t>
   </si>
   <si>
-    <t>/nas/teeselab/mark/databases/D_uniprot</t>
-  </si>
-  <si>
-    <t>add_user_subseqs</t>
-  </si>
-  <si>
-    <t>If "TRUE", user-based TMD or subsequences will be added from an external file (e.g. List12_SE_seqs).</t>
+    <t>/nas/teeselab/mark/databases/D_uniprot/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -931,16 +979,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <fill>
         <patternFill>
@@ -1080,9 +1121,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1120,9 +1161,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1155,26 +1196,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1207,26 +1231,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1400,23 +1407,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="85.5703125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>59</v>
@@ -1427,7 +1434,7 @@
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="53"/>
@@ -1437,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="37">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="C3" s="54" t="s">
         <v>9</v>
@@ -1470,235 +1477,229 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>93</v>
+        <v>190</v>
       </c>
       <c r="B7" s="39"/>
       <c r="C7" s="55"/>
     </row>
     <row r="8" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>98</v>
+        <v>176</v>
       </c>
       <c r="B8" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="56" t="s">
-        <v>14</v>
-      </c>
+      <c r="C8" s="56"/>
     </row>
     <row r="9" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>99</v>
+        <v>177</v>
       </c>
       <c r="B9" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="68" t="s">
-        <v>13</v>
-      </c>
+      <c r="C9" s="68"/>
     </row>
     <row r="10" spans="1:3" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="32"/>
+    </row>
+    <row r="11" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="B14" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="62"/>
+      <c r="C16" s="62"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="41"/>
+      <c r="C17" s="57"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="70" t="s">
+      <c r="B18" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="56" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="B12" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="B13" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="62"/>
-      <c r="C14" s="62"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="C18" s="65" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="66" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="62"/>
+      <c r="C20" s="62"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="57"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
-        <v>102</v>
-      </c>
-      <c r="B16" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="65" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="66" t="s">
-        <v>103</v>
-      </c>
-      <c r="B17" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="66" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
-      <c r="C18" s="62"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="59"/>
-    </row>
-    <row r="20" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B20" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B21" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>62</v>
-      </c>
+      <c r="B21" s="43"/>
+      <c r="C21" s="59"/>
     </row>
     <row r="22" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="62"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="62"/>
+    </row>
+    <row r="26" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="45"/>
+      <c r="C26" s="60"/>
+    </row>
+    <row r="27" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="62"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="62"/>
-    </row>
-    <row r="24" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="B27" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="61" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="62"/>
+      <c r="C30" s="62"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="60"/>
-    </row>
-    <row r="25" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="61" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="61" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="B27" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="61" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="62"/>
-      <c r="C28" s="62"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="48"/>
-      <c r="C29" s="27"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="B30" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>21</v>
-      </c>
+      <c r="B31" s="48"/>
+      <c r="C31" s="27"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B32" s="70" t="s">
         <v>8</v>
@@ -1709,7 +1710,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B33" s="70" t="s">
         <v>8</v>
@@ -1720,7 +1721,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B34" s="70" t="s">
         <v>8</v>
@@ -1731,7 +1732,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B35" s="70" t="s">
         <v>8</v>
@@ -1740,85 +1741,97 @@
         <v>21</v>
       </c>
     </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B6 B36:B1048576">
-    <cfRule type="containsText" dxfId="17" priority="124" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="B1 B6 B38:B1048576">
+    <cfRule type="containsText" dxfId="16" priority="170" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="containsText" dxfId="15" priority="168" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="containsText" dxfId="14" priority="167" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25">
+    <cfRule type="containsText" dxfId="13" priority="166" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="containsText" dxfId="12" priority="165" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:B37 B27 B29 B11:B12">
+    <cfRule type="containsText" dxfId="11" priority="164" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
+    <cfRule type="containsText" dxfId="10" priority="154" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="containsText" dxfId="9" priority="97" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="containsText" dxfId="8" priority="88" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="containsText" dxfId="16" priority="122" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="7" priority="18" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="containsText" dxfId="15" priority="121" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="6" priority="16" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
-    <cfRule type="containsText" dxfId="14" priority="120" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="13" priority="119" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30:B35 B25 B27 B8:B9">
-    <cfRule type="containsText" dxfId="12" priority="118" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="B8:B10">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26">
-    <cfRule type="containsText" dxfId="11" priority="108" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B26)))</formula>
+  <conditionalFormatting sqref="B22:B23 B19">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22">
-    <cfRule type="containsText" dxfId="10" priority="51" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B10">
-    <cfRule type="containsText" dxfId="9" priority="42" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="8" priority="17" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
-    <cfRule type="containsText" dxfId="7" priority="16" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B12)))</formula>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1828,22 +1841,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="61.28515625" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="71" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>59</v>
@@ -1854,13 +1867,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" t="s">
         <v>157</v>
-      </c>
-      <c r="B2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1868,7 +1881,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1876,7 +1889,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1884,7 +1897,7 @@
         <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1892,7 +1905,7 @@
         <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
         <v>73</v>
@@ -1903,7 +1916,7 @@
         <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="C7" t="s">
         <v>71</v>
@@ -1911,62 +1924,135 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B10" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="C11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" s="39"/>
+      <c r="C13" s="55"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" t="s">
+        <v>203</v>
+      </c>
+      <c r="C14" t="s">
         <v>167</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>174</v>
+      </c>
+      <c r="B16" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B18" s="39"/>
+      <c r="C18" s="55"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>183</v>
+      </c>
+      <c r="B20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>180</v>
+      </c>
+      <c r="B21" t="s">
         <v>185</v>
       </c>
-      <c r="C12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" t="s">
-        <v>183</v>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>187</v>
+      </c>
+      <c r="B23" t="s">
+        <v>188</v>
+      </c>
+      <c r="C23" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1979,10 +2065,10 @@
   <dimension ref="A1:C95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.42578125" customWidth="1"/>
     <col min="2" max="2" width="31" style="47" customWidth="1"/>
@@ -1991,7 +2077,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>59</v>
@@ -2062,8 +2148,8 @@
       <c r="A9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="40" t="b">
-        <v>0</v>
+      <c r="B9" s="40" t="s">
+        <v>7</v>
       </c>
       <c r="C9" s="56"/>
     </row>
@@ -2089,8 +2175,8 @@
       <c r="A12" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="40" t="b">
-        <v>0</v>
+      <c r="B12" s="40" t="s">
+        <v>7</v>
       </c>
       <c r="C12" s="56"/>
     </row>
@@ -2099,7 +2185,7 @@
         <v>49</v>
       </c>
       <c r="B13" s="40">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="C13" s="56" t="s">
         <v>61</v>
@@ -2128,7 +2214,7 @@
         <v>52</v>
       </c>
       <c r="B16" s="40">
-        <v>20000</v>
+        <v>3000</v>
       </c>
       <c r="C16" s="56"/>
     </row>
@@ -2156,47 +2242,47 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B20" s="41"/>
       <c r="C20" s="57"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B21" s="42" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B22" s="42" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B23" s="42" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B24" s="42" t="s">
         <v>7</v>
@@ -2205,18 +2291,18 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B25" s="42">
         <v>12</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B26" s="42">
         <v>4</v>
@@ -2225,7 +2311,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B27" s="42">
         <v>4</v>
@@ -2234,40 +2320,40 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B28" s="42" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B29" s="42">
         <v>0.4</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B30" s="42">
         <v>1</v>
       </c>
       <c r="C30" s="58" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B31" s="42" t="s">
         <v>7</v>
@@ -2276,7 +2362,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B32" s="42" t="s">
         <v>8</v>
@@ -2285,7 +2371,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B33" s="42">
         <v>10</v>
@@ -2294,7 +2380,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B34" s="42">
         <v>10</v>
@@ -2303,7 +2389,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B35" s="42" t="s">
         <v>32</v>
@@ -2312,13 +2398,13 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B36" s="42" t="s">
         <v>33</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2327,14 +2413,14 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="71" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B38" s="72"/>
       <c r="C38" s="73"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="74" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B39" s="75" t="b">
         <v>0</v>
@@ -2343,7 +2429,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B40" s="75" t="s">
         <v>32</v>
@@ -2352,7 +2438,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="74" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B41" s="75" t="s">
         <v>33</v>
@@ -2361,7 +2447,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="74" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B42" s="75">
         <v>2</v>
@@ -2370,7 +2456,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="74" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B43" s="75">
         <v>2</v>
@@ -2379,7 +2465,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="74" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B44" s="75">
         <v>0.4</v>
@@ -2388,7 +2474,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B45" s="75">
         <v>0.3</v>
@@ -2397,7 +2483,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B46" s="75">
         <v>0.3</v>
@@ -2406,7 +2492,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="74" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B47" s="75" t="s">
         <v>8</v>
@@ -2415,7 +2501,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B48" s="75">
         <v>20</v>
@@ -2424,7 +2510,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B49" s="75" t="s">
         <v>34</v>
@@ -2433,7 +2519,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="74" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B50" s="75">
         <v>1.1000000000000001</v>
@@ -2442,7 +2528,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B51" s="75">
         <v>0</v>
@@ -2451,7 +2537,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="74" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B52" s="75">
         <v>0</v>
@@ -2460,7 +2546,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="74" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B53" s="75" t="s">
         <v>8</v>
@@ -2554,7 +2640,7 @@
     </row>
     <row r="65" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B65" s="46">
         <v>20</v>
@@ -2653,7 +2739,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B76" s="46">
         <v>0.5</v>
@@ -2662,7 +2748,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B77" s="46">
         <v>1.75</v>
@@ -2759,7 +2845,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B89" s="49" t="s">
         <v>48</v>
@@ -2802,7 +2888,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B95" s="51" t="s">
         <v>33</v>

</xml_diff>